<commit_message>
receivers list added and PDF conversion rectified
</commit_message>
<xml_diff>
--- a/senders.xlsx
+++ b/senders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603C7C99-1FEE-420F-83DA-3913F94F912D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA90515A-21E9-4AC4-A46C-B0A888835A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="4980" windowWidth="21600" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
+    <workbookView xWindow="38460" yWindow="2595" windowWidth="15375" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,57 +399,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE00F2A-6AFA-4280-80FE-507041712647}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{79872A69-DE12-4F94-9F53-D6EDBB3CE5BF}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{0CF3EC1C-65AE-48BF-BBBB-E6049D6B865C}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{195BD25E-F2E6-459C-BB04-DA5B89DAE536}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{C1BF841C-B7D2-44E2-9B34-E6F753BA837F}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{79872A69-DE12-4F94-9F53-D6EDBB3CE5BF}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{0CF3EC1C-65AE-48BF-BBBB-E6049D6B865C}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{195BD25E-F2E6-459C-BB04-DA5B89DAE536}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{C1BF841C-B7D2-44E2-9B34-E6F753BA837F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
integrated third party client json and authentication
</commit_message>
<xml_diff>
--- a/senders.xlsx
+++ b/senders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter Local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA90515A-21E9-4AC4-A46C-B0A888835A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3760674-F279-49B0-86FD-F79943725485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38460" yWindow="2595" windowWidth="15375" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
+    <workbookView xWindow="39045" yWindow="6810" windowWidth="15375" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>bacchan.amit69@rekha.com</t>
-  </si>
-  <si>
-    <t>testedBrat@yahoo.com</t>
-  </si>
-  <si>
-    <t>pirates009@hotmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+  <si>
+    <t>uwtsjgxgxgk42@gmail.com</t>
+  </si>
+  <si>
+    <t>kdhuhfhfi38@gmail.com</t>
+  </si>
+  <si>
+    <t>kfhhfhfbc@gmail.com</t>
+  </si>
+  <si>
+    <t>jyretikdgdhl@gmail.com</t>
+  </si>
+  <si>
+    <t>guuofkhc@gmail.com</t>
+  </si>
+  <si>
+    <t>aass1122</t>
   </si>
 </sst>
 </file>
@@ -52,12 +58,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,17 +80,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE00F2A-6AFA-4280-80FE-507041712647}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,33 +428,47 @@
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{79872A69-DE12-4F94-9F53-D6EDBB3CE5BF}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{0CF3EC1C-65AE-48BF-BBBB-E6049D6B865C}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{195BD25E-F2E6-459C-BB04-DA5B89DAE536}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{C1BF841C-B7D2-44E2-9B34-E6F753BA837F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverted PDF file and changed randomize func
</commit_message>
<xml_diff>
--- a/senders.xlsx
+++ b/senders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3760674-F279-49B0-86FD-F79943725485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C60C71-49E3-4E7C-8550-BBE582D3BB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39045" yWindow="6810" windowWidth="15375" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,31 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>uwtsjgxgxgk42@gmail.com</t>
+    <t>emmanuelturner41@gmail.com</t>
   </si>
   <si>
-    <t>kdhuhfhfi38@gmail.com</t>
-  </si>
-  <si>
-    <t>kfhhfhfbc@gmail.com</t>
-  </si>
-  <si>
-    <t>jyretikdgdhl@gmail.com</t>
-  </si>
-  <si>
-    <t>guuofkhc@gmail.com</t>
-  </si>
-  <si>
-    <t>aass1122</t>
+    <t>wwkkk#$1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +50,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,14 +92,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,59 +415,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE00F2A-6AFA-4280-80FE-507041712647}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{613B3D1A-949F-44C6-A066-E64AA21BBFC3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>